<commit_message>
added Quality info dummy data + chart example in 3_Quality.py
</commit_message>
<xml_diff>
--- a/data/Dummy_Data.xlsx
+++ b/data/Dummy_Data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivelin.Hristov\source\repos\londemo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddimit01\Desktop\London Reporting Demo\londemo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0429202A-BA81-4421-93D3-869FE21B8694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DBECF5-7474-4D76-8E17-E4D6A2C258C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="16080" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_data" sheetId="1" r:id="rId1"/>
     <sheet name="relative_metric" sheetId="2" r:id="rId2"/>
     <sheet name="demographic" sheetId="3" r:id="rId3"/>
-    <sheet name="targets" sheetId="4" r:id="rId4"/>
+    <sheet name="Quality" sheetId="5" r:id="rId4"/>
+    <sheet name="targets" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">daily_data!$A$1:$X$508</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3753" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3784" uniqueCount="97">
   <si>
     <t>Country_Code</t>
   </si>
@@ -292,6 +293,45 @@
   <si>
     <t>Refusals</t>
   </si>
+  <si>
+    <t>LOI_median</t>
+  </si>
+  <si>
+    <t>Flagg_50%_LOI</t>
+  </si>
+  <si>
+    <t>Flagg_200%_LOI</t>
+  </si>
+  <si>
+    <t>SL%</t>
+  </si>
+  <si>
+    <t>NR%</t>
+  </si>
+  <si>
+    <t>NR%_Max</t>
+  </si>
+  <si>
+    <t>NR%_95th_percentile</t>
+  </si>
+  <si>
+    <t>KPI Cards</t>
+  </si>
+  <si>
+    <t>LOI Median</t>
+  </si>
+  <si>
+    <t>NR% Aveage</t>
+  </si>
+  <si>
+    <t>SL% Average</t>
+  </si>
+  <si>
+    <t>Data Quality Issues</t>
+  </si>
+  <si>
+    <t>Sl_40%+</t>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +341,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0%"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +361,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -516,10 +563,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -658,9 +706,16 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -965,15 +1020,15 @@
   </sheetPr>
   <dimension ref="A1:X509"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="30" customWidth="1"/>
     <col min="6" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -39632,8 +39687,8 @@
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39754,19 +39809,19 @@
       </c>
       <c r="K3" s="8">
         <f ca="1">demographic!G3-_xlfn.XLOOKUP($A3,targets!$B:$B,targets!I:I)</f>
-        <v>0.12461538461538463</v>
+        <v>3.4615384615384659E-2</v>
       </c>
       <c r="L3" s="8">
         <f ca="1">demographic!H3-_xlfn.XLOOKUP($A3,targets!$B:$B,targets!J:J)</f>
-        <v>-0.31461538461538463</v>
+        <v>-0.18461538461538463</v>
       </c>
       <c r="M3" s="8">
         <f ca="1">demographic!I3-_xlfn.XLOOKUP($A3,targets!$B:$B,targets!K:K)</f>
-        <v>4.4871794871794879E-2</v>
+        <v>2.4871794871794861E-2</v>
       </c>
       <c r="N3" s="8">
         <f ca="1">demographic!J3-_xlfn.XLOOKUP($A3,targets!$B:$B,targets!L:L)</f>
-        <v>0.14512820512820512</v>
+        <v>0.12512820512820511</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -39811,15 +39866,15 @@
       </c>
       <c r="K4" s="8">
         <f ca="1">demographic!G4-_xlfn.XLOOKUP($A4,targets!$B:$B,targets!I:I)</f>
-        <v>0.13904761904761903</v>
+        <v>0.10904761904761906</v>
       </c>
       <c r="L4" s="8">
         <f ca="1">demographic!H4-_xlfn.XLOOKUP($A4,targets!$B:$B,targets!J:J)</f>
-        <v>-0.29904761904761901</v>
+        <v>-0.21904761904761907</v>
       </c>
       <c r="M4" s="8">
         <f ca="1">demographic!I4-_xlfn.XLOOKUP($A4,targets!$B:$B,targets!K:K)</f>
-        <v>5.4761904761904762E-2</v>
+        <v>4.761904761904745E-3</v>
       </c>
       <c r="N4" s="8">
         <f ca="1">demographic!J4-_xlfn.XLOOKUP($A4,targets!$B:$B,targets!L:L)</f>
@@ -39868,19 +39923,19 @@
       </c>
       <c r="K5" s="8">
         <f ca="1">demographic!G5-_xlfn.XLOOKUP($A5,targets!$B:$B,targets!I:I)</f>
-        <v>0.10853617021276596</v>
+        <v>9.8936170212765961E-2</v>
       </c>
       <c r="L5" s="8">
         <f ca="1">demographic!H5-_xlfn.XLOOKUP($A5,targets!$B:$B,targets!J:J)</f>
-        <v>-0.25047659574468084</v>
+        <v>-0.21127659574468086</v>
       </c>
       <c r="M5" s="8">
         <f ca="1">demographic!I5-_xlfn.XLOOKUP($A5,targets!$B:$B,targets!K:K)</f>
-        <v>3.1489361702127655E-2</v>
+        <v>-8.5106382978723527E-3</v>
       </c>
       <c r="N5" s="8">
         <f ca="1">demographic!J5-_xlfn.XLOOKUP($A5,targets!$B:$B,targets!L:L)</f>
-        <v>0.11045106382978724</v>
+        <v>0.12085106382978725</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -39925,19 +39980,19 @@
       </c>
       <c r="K6" s="8">
         <f ca="1">demographic!G6-_xlfn.XLOOKUP($A6,targets!$B:$B,targets!I:I)</f>
-        <v>0.11096618357487925</v>
+        <v>0.14096618357487922</v>
       </c>
       <c r="L6" s="8">
         <f ca="1">demographic!H6-_xlfn.XLOOKUP($A6,targets!$B:$B,targets!J:J)</f>
-        <v>-0.27159420289855074</v>
+        <v>-0.31159420289855072</v>
       </c>
       <c r="M6" s="8">
         <f ca="1">demographic!I6-_xlfn.XLOOKUP($A6,targets!$B:$B,targets!K:K)</f>
-        <v>1.7729468599033821E-2</v>
+        <v>5.7729468599033829E-2</v>
       </c>
       <c r="N6" s="8">
         <f ca="1">demographic!J6-_xlfn.XLOOKUP($A6,targets!$B:$B,targets!L:L)</f>
-        <v>0.1428985507246377</v>
+        <v>0.1128985507246377</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -39986,15 +40041,15 @@
       </c>
       <c r="L7" s="8">
         <f ca="1">demographic!H7-_xlfn.XLOOKUP($A7,targets!$B:$B,targets!J:J)</f>
-        <v>-0.27770833333333333</v>
+        <v>-0.28770833333333334</v>
       </c>
       <c r="M7" s="8">
         <f ca="1">demographic!I7-_xlfn.XLOOKUP($A7,targets!$B:$B,targets!K:K)</f>
-        <v>1.833333333333334E-2</v>
+        <v>8.3333333333333315E-3</v>
       </c>
       <c r="N7" s="8">
         <f ca="1">demographic!J7-_xlfn.XLOOKUP($A7,targets!$B:$B,targets!L:L)</f>
-        <v>0.113125</v>
+        <v>0.13312499999999999</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40039,19 +40094,19 @@
       </c>
       <c r="K8" s="8">
         <f ca="1">demographic!G8-_xlfn.XLOOKUP($A8,targets!$B:$B,targets!I:I)</f>
-        <v>7.3737373737373768E-2</v>
+        <v>3.3737373737373733E-2</v>
       </c>
       <c r="L8" s="8">
         <f ca="1">demographic!H8-_xlfn.XLOOKUP($A8,targets!$B:$B,targets!J:J)</f>
-        <v>-0.21272727272727274</v>
+        <v>-0.17272727272727276</v>
       </c>
       <c r="M8" s="8">
         <f ca="1">demographic!I8-_xlfn.XLOOKUP($A8,targets!$B:$B,targets!K:K)</f>
-        <v>-3.0303030303030498E-3</v>
+        <v>1.6969696969696968E-2</v>
       </c>
       <c r="N8" s="8">
         <f ca="1">demographic!J8-_xlfn.XLOOKUP($A8,targets!$B:$B,targets!L:L)</f>
-        <v>0.14202020202020202</v>
+        <v>0.12202020202020201</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40096,19 +40151,19 @@
       </c>
       <c r="K9" s="8">
         <f ca="1">demographic!G9-_xlfn.XLOOKUP($A9,targets!$B:$B,targets!I:I)</f>
-        <v>8.4096916299559454E-2</v>
+        <v>0.14409691629955945</v>
       </c>
       <c r="L9" s="8">
         <f ca="1">demographic!H9-_xlfn.XLOOKUP($A9,targets!$B:$B,targets!J:J)</f>
-        <v>-0.24378854625550658</v>
+        <v>-0.30378854625550655</v>
       </c>
       <c r="M9" s="8">
         <f ca="1">demographic!I9-_xlfn.XLOOKUP($A9,targets!$B:$B,targets!K:K)</f>
-        <v>1.7048458149779733E-2</v>
+        <v>5.7048458149779741E-2</v>
       </c>
       <c r="N9" s="8">
         <f ca="1">demographic!J9-_xlfn.XLOOKUP($A9,targets!$B:$B,targets!L:L)</f>
-        <v>0.1426431718061674</v>
+        <v>0.10264317180616739</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40153,11 +40208,11 @@
       </c>
       <c r="K10" s="8">
         <f ca="1">demographic!G10-_xlfn.XLOOKUP($A10,targets!$B:$B,targets!I:I)</f>
-        <v>0.12795918367346937</v>
+        <v>0.11795918367346936</v>
       </c>
       <c r="L10" s="8">
         <f ca="1">demographic!H10-_xlfn.XLOOKUP($A10,targets!$B:$B,targets!J:J)</f>
-        <v>-0.26571428571428568</v>
+        <v>-0.24571428571428575</v>
       </c>
       <c r="M10" s="8">
         <f ca="1">demographic!I10-_xlfn.XLOOKUP($A10,targets!$B:$B,targets!K:K)</f>
@@ -40165,64 +40220,64 @@
       </c>
       <c r="N10" s="8">
         <f ca="1">demographic!J10-_xlfn.XLOOKUP($A10,targets!$B:$B,targets!L:L)</f>
-        <v>0.12897959183673469</v>
+        <v>0.11897959183673469</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B11" s="5">
         <f>SUMIF(daily_data!B:B,"="&amp;A11,daily_data!I:I)</f>
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="C11" s="5">
         <f>SUMIFS(daily_data!P:P,daily_data!$B:$B,"="&amp;demographic!$A11)</f>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="D11" s="5">
         <f>SUMIFS(daily_data!Q:Q,daily_data!$B:$B,"="&amp;demographic!$A11)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E11" s="5">
         <f>SUMIFS(daily_data!R:R,daily_data!$B:$B,"="&amp;demographic!$A11)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5">
         <f>SUMIFS(daily_data!S:S,daily_data!$B:$B,"="&amp;demographic!$A11)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="6" t="e">
+        <v>34</v>
+      </c>
+      <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="6" t="e">
+        <v>0.40119760479041916</v>
+      </c>
+      <c r="H11" s="6">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="6" t="e">
+        <v>0.22754491017964071</v>
+      </c>
+      <c r="I11" s="6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="6" t="e">
+        <v>0.16766467065868262</v>
+      </c>
+      <c r="J11" s="6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="8" t="e">
-        <f>demographic!G11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!I:I)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L11" s="8" t="e">
-        <f>demographic!H11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!J:J)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="8" t="e">
-        <f>demographic!I11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!K:K)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="8" t="e">
-        <f>demographic!J11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!L:L)</f>
-        <v>#DIV/0!</v>
+        <v>0.20359281437125748</v>
+      </c>
+      <c r="K11" s="8">
+        <f ca="1">demographic!G11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!I:I)</f>
+        <v>8.1197604790419153E-2</v>
+      </c>
+      <c r="L11" s="8">
+        <f ca="1">demographic!H11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!J:J)</f>
+        <v>-0.18245508982035927</v>
+      </c>
+      <c r="M11" s="8">
+        <f ca="1">demographic!I11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!K:K)</f>
+        <v>-1.2335329341317369E-2</v>
+      </c>
+      <c r="N11" s="8">
+        <f ca="1">demographic!J11-_xlfn.XLOOKUP($A11,targets!$B:$B,targets!L:L)</f>
+        <v>0.11359281437125748</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40267,19 +40322,19 @@
       </c>
       <c r="K12" s="8">
         <f ca="1">demographic!G12-_xlfn.XLOOKUP($A12,targets!$B:$B,targets!I:I)</f>
-        <v>0.1325974025974026</v>
+        <v>0.10259740259740263</v>
       </c>
       <c r="L12" s="8">
         <f ca="1">demographic!H12-_xlfn.XLOOKUP($A12,targets!$B:$B,targets!J:J)</f>
-        <v>-0.27952380952380951</v>
+        <v>-0.24952380952380954</v>
       </c>
       <c r="M12" s="8">
         <f ca="1">demographic!I12-_xlfn.XLOOKUP($A12,targets!$B:$B,targets!K:K)</f>
-        <v>1.3463203463203455E-2</v>
+        <v>2.3463203463203464E-2</v>
       </c>
       <c r="N12" s="8">
         <f ca="1">demographic!J12-_xlfn.XLOOKUP($A12,targets!$B:$B,targets!L:L)</f>
-        <v>0.13346320346320345</v>
+        <v>0.12346320346320346</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40324,11 +40379,11 @@
       </c>
       <c r="K13" s="8">
         <f ca="1">demographic!G13-_xlfn.XLOOKUP($A13,targets!$B:$B,targets!I:I)</f>
-        <v>0.15000000000000002</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="L13" s="8">
         <f ca="1">demographic!H13-_xlfn.XLOOKUP($A13,targets!$B:$B,targets!J:J)</f>
-        <v>-0.30714285714285716</v>
+        <v>-0.28714285714285714</v>
       </c>
       <c r="M13" s="8">
         <f ca="1">demographic!I13-_xlfn.XLOOKUP($A13,targets!$B:$B,targets!K:K)</f>
@@ -40336,7 +40391,7 @@
       </c>
       <c r="N13" s="8">
         <f ca="1">demographic!J13-_xlfn.XLOOKUP($A13,targets!$B:$B,targets!L:L)</f>
-        <v>0.14571428571428571</v>
+        <v>0.1357142857142857</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40381,19 +40436,19 @@
       </c>
       <c r="K14" s="8">
         <f ca="1">demographic!G14-_xlfn.XLOOKUP($A14,targets!$B:$B,targets!I:I)</f>
-        <v>0.12223463687150837</v>
+        <v>7.1567970204841735E-2</v>
       </c>
       <c r="L14" s="8">
         <f ca="1">demographic!H14-_xlfn.XLOOKUP($A14,targets!$B:$B,targets!J:J)</f>
-        <v>-0.33430912476722541</v>
+        <v>-0.244975791433892</v>
       </c>
       <c r="M14" s="8">
         <f ca="1">demographic!I14-_xlfn.XLOOKUP($A14,targets!$B:$B,targets!K:K)</f>
-        <v>4.4864059590316557E-2</v>
+        <v>3.5530726256983225E-2</v>
       </c>
       <c r="N14" s="8">
         <f ca="1">demographic!J14-_xlfn.XLOOKUP($A14,targets!$B:$B,targets!L:L)</f>
-        <v>0.16721042830540037</v>
+        <v>0.13787709497206702</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40438,19 +40493,19 @@
       </c>
       <c r="K15" s="8">
         <f ca="1">demographic!G15-_xlfn.XLOOKUP($A15,targets!$B:$B,targets!I:I)</f>
-        <v>0.1522346368715084</v>
+        <v>0.11223463687150842</v>
       </c>
       <c r="L15" s="8">
         <f ca="1">demographic!H15-_xlfn.XLOOKUP($A15,targets!$B:$B,targets!J:J)</f>
-        <v>-0.28681564245810054</v>
+        <v>-0.33681564245810058</v>
       </c>
       <c r="M15" s="8">
         <f ca="1">demographic!I15-_xlfn.XLOOKUP($A15,targets!$B:$B,targets!K:K)</f>
-        <v>1.787709497206702E-2</v>
+        <v>6.7877094972067037E-2</v>
       </c>
       <c r="N15" s="8">
         <f ca="1">demographic!J15-_xlfn.XLOOKUP($A15,targets!$B:$B,targets!L:L)</f>
-        <v>0.11670391061452515</v>
+        <v>0.15670391061452515</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40459,7 +40514,7 @@
       </c>
       <c r="B16" s="13">
         <f>SUM(B3:B15)</f>
-        <v>2377</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -40534,11 +40589,11 @@
       </c>
       <c r="G22" s="6">
         <f ca="1">demographic!E22-_xlfn.XLOOKUP($A22,targets!$B:$B,targets!O:O)</f>
-        <v>-3.2307692307692371E-2</v>
+        <v>-1.2307692307692353E-2</v>
       </c>
       <c r="H22" s="6">
         <f ca="1">demographic!F22-_xlfn.XLOOKUP($A22,targets!$B:$B,targets!P:P)</f>
-        <v>3.2307692307692315E-2</v>
+        <v>1.2307692307692353E-2</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40567,11 +40622,11 @@
       </c>
       <c r="G23" s="6">
         <f ca="1">demographic!E23-_xlfn.XLOOKUP($A23,targets!$B:$B,targets!O:O)</f>
-        <v>-9.5238095238095233E-2</v>
+        <v>0.10476190476190472</v>
       </c>
       <c r="H23" s="6">
         <f ca="1">demographic!F23-_xlfn.XLOOKUP($A23,targets!$B:$B,targets!P:P)</f>
-        <v>9.5238095238095233E-2</v>
+        <v>-0.10476190476190472</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40600,11 +40655,11 @@
       </c>
       <c r="G24" s="6">
         <f ca="1">demographic!E24-_xlfn.XLOOKUP($A24,targets!$B:$B,targets!O:O)</f>
-        <v>0.19723404255319149</v>
+        <v>0.30683404255319152</v>
       </c>
       <c r="H24" s="6">
         <f ca="1">demographic!F24-_xlfn.XLOOKUP($A24,targets!$B:$B,targets!P:P)</f>
-        <v>-0.19723404255319155</v>
+        <v>-0.30683404255319147</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40633,11 +40688,11 @@
       </c>
       <c r="G25" s="6">
         <f ca="1">demographic!E25-_xlfn.XLOOKUP($A25,targets!$B:$B,targets!O:O)</f>
-        <v>-5.140096618357487E-2</v>
+        <v>2.8599033816425146E-2</v>
       </c>
       <c r="H25" s="6">
         <f ca="1">demographic!F25-_xlfn.XLOOKUP($A25,targets!$B:$B,targets!P:P)</f>
-        <v>5.1400966183574925E-2</v>
+        <v>-2.8599033816425146E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40666,11 +40721,11 @@
       </c>
       <c r="G26" s="6">
         <f ca="1">demographic!E26-_xlfn.XLOOKUP($A26,targets!$B:$B,targets!O:O)</f>
-        <v>0.28041666666666665</v>
+        <v>0.27041666666666664</v>
       </c>
       <c r="H26" s="6">
         <f ca="1">demographic!F26-_xlfn.XLOOKUP($A26,targets!$B:$B,targets!P:P)</f>
-        <v>-0.2804166666666667</v>
+        <v>-0.27041666666666669</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40699,11 +40754,11 @@
       </c>
       <c r="G27" s="6">
         <f ca="1">demographic!E27-_xlfn.XLOOKUP($A27,targets!$B:$B,targets!O:O)</f>
-        <v>0.27</v>
+        <v>0.16999999999999998</v>
       </c>
       <c r="H27" s="6">
         <f ca="1">demographic!F27-_xlfn.XLOOKUP($A27,targets!$B:$B,targets!P:P)</f>
-        <v>-0.27</v>
+        <v>-0.17000000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40732,11 +40787,11 @@
       </c>
       <c r="G28" s="6">
         <f ca="1">demographic!E28-_xlfn.XLOOKUP($A28,targets!$B:$B,targets!O:O)</f>
-        <v>0.17625550660792955</v>
+        <v>-5.3744493392070436E-2</v>
       </c>
       <c r="H28" s="6">
         <f ca="1">demographic!F28-_xlfn.XLOOKUP($A28,targets!$B:$B,targets!P:P)</f>
-        <v>-0.17625550660792955</v>
+        <v>5.3744493392070436E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40864,11 +40919,11 @@
       </c>
       <c r="G32" s="6">
         <f ca="1">demographic!E32-_xlfn.XLOOKUP($A32,targets!$B:$B,targets!O:O)</f>
-        <v>8.4285714285714242E-2</v>
+        <v>0.26428571428571423</v>
       </c>
       <c r="H32" s="6">
         <f ca="1">demographic!F32-_xlfn.XLOOKUP($A32,targets!$B:$B,targets!P:P)</f>
-        <v>-8.4285714285714242E-2</v>
+        <v>-0.26428571428571429</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40897,11 +40952,11 @@
       </c>
       <c r="G33" s="6">
         <f ca="1">demographic!E33-_xlfn.XLOOKUP($A33,targets!$B:$B,targets!O:O)</f>
-        <v>-5.111359404096838E-2</v>
+        <v>0.28888640595903159</v>
       </c>
       <c r="H33" s="6">
         <f ca="1">demographic!F33-_xlfn.XLOOKUP($A33,targets!$B:$B,targets!P:P)</f>
-        <v>5.1113594040968324E-2</v>
+        <v>-0.28888640595903164</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -40930,11 +40985,11 @@
       </c>
       <c r="G34" s="6">
         <f ca="1">demographic!E34-_xlfn.XLOOKUP($A34,targets!$B:$B,targets!O:O)</f>
-        <v>-8.3966480446927338E-2</v>
+        <v>4.603351955307261E-2</v>
       </c>
       <c r="H34" s="6">
         <f ca="1">demographic!F34-_xlfn.XLOOKUP($A34,targets!$B:$B,targets!P:P)</f>
-        <v>8.3966480446927394E-2</v>
+        <v>-4.6033519553072666E-2</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41037,15 +41092,15 @@
       </c>
       <c r="I40" s="6">
         <f ca="1">demographic!F40-_xlfn.XLOOKUP($A40,targets!$B:$B,targets!T:T)</f>
-        <v>0.19846153846153847</v>
+        <v>7.8461538461538471E-2</v>
       </c>
       <c r="J40" s="6">
         <f ca="1">demographic!G40-_xlfn.XLOOKUP($A40,targets!$B:$B,targets!U:U)</f>
-        <v>-9.0769230769230824E-2</v>
+        <v>9.9230769230769234E-2</v>
       </c>
       <c r="K40" s="6">
         <f ca="1">demographic!H40-_xlfn.XLOOKUP($A40,targets!$B:$B,targets!V:V)</f>
-        <v>-0.1076923076923077</v>
+        <v>-0.1776923076923077</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41082,15 +41137,15 @@
       </c>
       <c r="I41" s="6">
         <f ca="1">demographic!F41-_xlfn.XLOOKUP($A41,targets!$B:$B,targets!T:T)</f>
-        <v>0.13190476190476189</v>
+        <v>0.25190476190476191</v>
       </c>
       <c r="J41" s="6">
         <f ca="1">demographic!G41-_xlfn.XLOOKUP($A41,targets!$B:$B,targets!U:U)</f>
-        <v>8.2380952380952444E-2</v>
+        <v>-0.18761904761904757</v>
       </c>
       <c r="K41" s="6">
         <f ca="1">demographic!H41-_xlfn.XLOOKUP($A41,targets!$B:$B,targets!V:V)</f>
-        <v>-0.21428571428571427</v>
+        <v>-6.4285714285714279E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41127,11 +41182,11 @@
       </c>
       <c r="I42" s="6">
         <f ca="1">demographic!F42-_xlfn.XLOOKUP($A42,targets!$B:$B,targets!T:T)</f>
-        <v>0.16598297872340423</v>
+        <v>-1.4017021276595765E-2</v>
       </c>
       <c r="J42" s="6">
         <f ca="1">demographic!G42-_xlfn.XLOOKUP($A42,targets!$B:$B,targets!U:U)</f>
-        <v>1.8272340425531941E-2</v>
+        <v>0.19827234042553188</v>
       </c>
       <c r="K42" s="6">
         <f ca="1">demographic!H42-_xlfn.XLOOKUP($A42,targets!$B:$B,targets!V:V)</f>
@@ -41172,15 +41227,15 @@
       </c>
       <c r="I43" s="6">
         <f ca="1">demographic!F43-_xlfn.XLOOKUP($A43,targets!$B:$B,targets!T:T)</f>
-        <v>-2.1835748792270515E-2</v>
+        <v>-6.1835748792270551E-2</v>
       </c>
       <c r="J43" s="6">
         <f ca="1">demographic!G43-_xlfn.XLOOKUP($A43,targets!$B:$B,targets!U:U)</f>
-        <v>0.13521739130434779</v>
+        <v>0.23521739130434777</v>
       </c>
       <c r="K43" s="6">
         <f ca="1">demographic!H43-_xlfn.XLOOKUP($A43,targets!$B:$B,targets!V:V)</f>
-        <v>-0.11338164251207729</v>
+        <v>-0.17338164251207733</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41217,15 +41272,15 @@
       </c>
       <c r="I44" s="6">
         <f ca="1">demographic!F44-_xlfn.XLOOKUP($A44,targets!$B:$B,targets!T:T)</f>
-        <v>3.8541666666666696E-2</v>
+        <v>0.11854166666666668</v>
       </c>
       <c r="J44" s="6">
         <f ca="1">demographic!G44-_xlfn.XLOOKUP($A44,targets!$B:$B,targets!U:U)</f>
-        <v>3.2916666666666594E-2</v>
+        <v>2.9166666666666785E-3</v>
       </c>
       <c r="K44" s="6">
         <f ca="1">demographic!H44-_xlfn.XLOOKUP($A44,targets!$B:$B,targets!V:V)</f>
-        <v>-7.1458333333333332E-2</v>
+        <v>-0.12145833333333332</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41262,15 +41317,15 @@
       </c>
       <c r="I45" s="6">
         <f ca="1">demographic!F45-_xlfn.XLOOKUP($A45,targets!$B:$B,targets!T:T)</f>
-        <v>3.4343434343434009E-3</v>
+        <v>0.24343434343434342</v>
       </c>
       <c r="J45" s="6">
         <f ca="1">demographic!G45-_xlfn.XLOOKUP($A45,targets!$B:$B,targets!U:U)</f>
-        <v>0.18060606060606055</v>
+        <v>-3.9393939393939426E-2</v>
       </c>
       <c r="K45" s="6">
         <f ca="1">demographic!H45-_xlfn.XLOOKUP($A45,targets!$B:$B,targets!V:V)</f>
-        <v>-0.18404040404040406</v>
+        <v>-0.20404040404040402</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41307,15 +41362,15 @@
       </c>
       <c r="I46" s="6">
         <f ca="1">demographic!F46-_xlfn.XLOOKUP($A46,targets!$B:$B,targets!T:T)</f>
-        <v>0.15361233480176212</v>
+        <v>3.612334801762096E-3</v>
       </c>
       <c r="J46" s="6">
         <f ca="1">demographic!G46-_xlfn.XLOOKUP($A46,targets!$B:$B,targets!U:U)</f>
-        <v>-9.6123348017621124E-2</v>
+        <v>0.1238766519823789</v>
       </c>
       <c r="K46" s="6">
         <f ca="1">demographic!H46-_xlfn.XLOOKUP($A46,targets!$B:$B,targets!V:V)</f>
-        <v>-5.7488986784140966E-2</v>
+        <v>-0.12748898678414097</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41352,15 +41407,15 @@
       </c>
       <c r="I47" s="6">
         <f ca="1">demographic!F47-_xlfn.XLOOKUP($A47,targets!$B:$B,targets!T:T)</f>
-        <v>0.22204081632653061</v>
+        <v>9.2040816326530606E-2</v>
       </c>
       <c r="J47" s="6">
         <f ca="1">demographic!G47-_xlfn.XLOOKUP($A47,targets!$B:$B,targets!U:U)</f>
-        <v>6.7346938775511012E-3</v>
+        <v>4.6734693877551026E-2</v>
       </c>
       <c r="K47" s="6">
         <f ca="1">demographic!H47-_xlfn.XLOOKUP($A47,targets!$B:$B,targets!V:V)</f>
-        <v>-0.2287755102040816</v>
+        <v>-0.13877551020408163</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41442,15 +41497,15 @@
       </c>
       <c r="I49" s="6">
         <f ca="1">demographic!F49-_xlfn.XLOOKUP($A49,targets!$B:$B,targets!T:T)</f>
-        <v>2.7662337662337666E-2</v>
+        <v>1.7662337662337657E-2</v>
       </c>
       <c r="J49" s="6">
         <f ca="1">demographic!G49-_xlfn.XLOOKUP($A49,targets!$B:$B,targets!U:U)</f>
-        <v>0.18575757575757579</v>
+        <v>9.5757575757575819E-2</v>
       </c>
       <c r="K49" s="6">
         <f ca="1">demographic!H49-_xlfn.XLOOKUP($A49,targets!$B:$B,targets!V:V)</f>
-        <v>-0.2134199134199134</v>
+        <v>-0.11341991341991343</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41487,15 +41542,15 @@
       </c>
       <c r="I50" s="6">
         <f ca="1">demographic!F50-_xlfn.XLOOKUP($A50,targets!$B:$B,targets!T:T)</f>
-        <v>9.4285714285714251E-2</v>
+        <v>0.11428571428571427</v>
       </c>
       <c r="J50" s="6">
         <f ca="1">demographic!G50-_xlfn.XLOOKUP($A50,targets!$B:$B,targets!U:U)</f>
-        <v>0</v>
+        <v>-4.9999999999999933E-2</v>
       </c>
       <c r="K50" s="6">
         <f ca="1">demographic!H50-_xlfn.XLOOKUP($A50,targets!$B:$B,targets!V:V)</f>
-        <v>-9.4285714285714278E-2</v>
+        <v>-6.4285714285714279E-2</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41536,11 +41591,11 @@
       </c>
       <c r="J51" s="6">
         <f ca="1">demographic!G51-_xlfn.XLOOKUP($A51,targets!$B:$B,targets!U:U)</f>
-        <v>-0.13911359404096835</v>
+        <v>-0.14978026070763506</v>
       </c>
       <c r="K51" s="6">
         <f ca="1">demographic!H51-_xlfn.XLOOKUP($A51,targets!$B:$B,targets!V:V)</f>
-        <v>-6.4521415270018617E-2</v>
+        <v>-5.385474860335196E-2</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41577,15 +41632,15 @@
       </c>
       <c r="I52" s="6">
         <f ca="1">demographic!F52-_xlfn.XLOOKUP($A52,targets!$B:$B,targets!T:T)</f>
-        <v>0.18960893854748601</v>
+        <v>-7.0391061452514003E-2</v>
       </c>
       <c r="J52" s="6">
         <f ca="1">demographic!G52-_xlfn.XLOOKUP($A52,targets!$B:$B,targets!U:U)</f>
-        <v>-0.11899441340782113</v>
+        <v>0.19100558659217881</v>
       </c>
       <c r="K52" s="6">
         <f ca="1">demographic!H52-_xlfn.XLOOKUP($A52,targets!$B:$B,targets!V:V)</f>
-        <v>-7.0614525139664805E-2</v>
+        <v>-0.12061452513966479</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41617,13 +41672,709 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63E2D99-6E5D-4B64-BC36-24FCB2929454}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="51">
+        <f ca="1">MEDIAN(D9:D21)</f>
+        <v>26.995485987035991</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="52">
+        <f ca="1">AVERAGE(G9:G21)</f>
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="52">
+        <f ca="1">AVERAGE(J9:J21)</f>
+        <v>0.10384615384615385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="53">
+        <f ca="1">SUM(E9:F21)+SUM(K9:K21)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A9,daily_data!I:I)</f>
+        <v>195</v>
+      </c>
+      <c r="C9" t="str">
+        <f>_xlfn.XLOOKUP(A9,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 2</v>
+      </c>
+      <c r="D9" s="51">
+        <f ca="1">RANDBETWEEN(12.5,24.5)*(RAND()+1)</f>
+        <v>29.529304144711581</v>
+      </c>
+      <c r="E9">
+        <f ca="1">ROUND((RANDBETWEEN(0,3)/100)*B9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f ca="1">ROUND((RANDBETWEEN(0,2)/100)*B9,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G9" s="52">
+        <f ca="1">RANDBETWEEN(3,35)/100</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H9">
+        <f ca="1">RANDBETWEEN(G9,75)</f>
+        <v>46</v>
+      </c>
+      <c r="I9">
+        <f ca="1">RANDBETWEEN(1,12)</f>
+        <v>5</v>
+      </c>
+      <c r="J9" s="52">
+        <f ca="1">RANDBETWEEN(3,18)/100</f>
+        <v>0.04</v>
+      </c>
+      <c r="K9">
+        <f ca="1">ROUND((RANDBETWEEN(2,5)/100)*J9*B9,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A10,daily_data!I:I)</f>
+        <v>210</v>
+      </c>
+      <c r="C10" t="str">
+        <f>_xlfn.XLOOKUP(A10,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 2</v>
+      </c>
+      <c r="D10" s="51">
+        <f t="shared" ref="D10:D21" ca="1" si="0">RANDBETWEEN(12.5,24.5)*(RAND()+1)</f>
+        <v>32.241424392108705</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E21" ca="1" si="1">ROUND((RANDBETWEEN(0,3)/100)*B10,0)</f>
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10:F21" ca="1" si="2">ROUND((RANDBETWEEN(0,2)/100)*B10,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="52">
+        <f t="shared" ref="G10:G21" ca="1" si="3">RANDBETWEEN(3,35)/100</f>
+        <v>0.31</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H21" ca="1" si="4">RANDBETWEEN(G10,75)</f>
+        <v>49</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:I21" ca="1" si="5">RANDBETWEEN(1,12)</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="52">
+        <f t="shared" ref="J10:J21" ca="1" si="6">RANDBETWEEN(3,18)/100</f>
+        <v>0.11</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K21" ca="1" si="7">ROUND((RANDBETWEEN(2,5)/100)*J10*B10,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A11,daily_data!I:I)</f>
+        <v>188</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.XLOOKUP(A11,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 2</v>
+      </c>
+      <c r="D11" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>36.686843509448359</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G11" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="J11" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.06</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A12,daily_data!I:I)</f>
+        <v>207</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.XLOOKUP(A12,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 4</v>
+      </c>
+      <c r="D12" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>19.826536856565642</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="J12" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A13,daily_data!I:I)</f>
+        <v>192</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.XLOOKUP(A13,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 1</v>
+      </c>
+      <c r="D13" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>22.817294677698399</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G13" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="J13" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.18</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A14,daily_data!I:I)</f>
+        <v>198</v>
+      </c>
+      <c r="C14" t="str">
+        <f>_xlfn.XLOOKUP(A14,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 2</v>
+      </c>
+      <c r="D14" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>27.907063386934006</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G14" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.13</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="J14" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A15,daily_data!I:I)</f>
+        <v>227</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xlfn.XLOOKUP(A15,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 1</v>
+      </c>
+      <c r="D15" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>36.780691086891878</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G15" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="J15" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.13</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A16,daily_data!I:I)</f>
+        <v>196</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xlfn.XLOOKUP(A16,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 1</v>
+      </c>
+      <c r="D16" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>33.582011097561363</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="J16" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.12</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A17,daily_data!I:I)</f>
+        <v>167</v>
+      </c>
+      <c r="C17" t="str">
+        <f>_xlfn.XLOOKUP(A17,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 3</v>
+      </c>
+      <c r="D17" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>20.945593326449561</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G17" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.12</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J17" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.11</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A18,daily_data!I:I)</f>
+        <v>231</v>
+      </c>
+      <c r="C18" t="str">
+        <f>_xlfn.XLOOKUP(A18,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 3</v>
+      </c>
+      <c r="D18" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>26.995485987035991</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G18" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ca="1" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="J18" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.03</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A19,daily_data!I:I)</f>
+        <v>175</v>
+      </c>
+      <c r="C19" t="str">
+        <f>_xlfn.XLOOKUP(A19,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 2</v>
+      </c>
+      <c r="D19" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>23.656552002009828</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.34</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="4"/>
+        <v>74</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="J19" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.06</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A20,daily_data!I:I)</f>
+        <v>179</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xlfn.XLOOKUP(A20,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 3</v>
+      </c>
+      <c r="D20" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>24.259229685575459</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.12</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="J20" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.12</v>
+      </c>
+      <c r="K20">
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="5">
+        <f>SUMIF(daily_data!B:B,"="&amp;A21,daily_data!I:I)</f>
+        <v>179</v>
+      </c>
+      <c r="C21" t="str">
+        <f>_xlfn.XLOOKUP(A21,daily_data!B:B,daily_data!D:D)</f>
+        <v>Group 4</v>
+      </c>
+      <c r="D21" s="51">
+        <f t="shared" ca="1" si="0"/>
+        <v>18.462658611323366</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G21" s="52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.13</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ca="1" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="J21" s="52">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.13</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="13">
+        <f>SUM(B9:B21)</f>
+        <v>2544</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -41725,75 +42476,75 @@
       </c>
       <c r="E2" s="5">
         <f t="shared" ref="E2:E14" ca="1" si="0">ROUND((RANDBETWEEN(25,35)/100)*C2,0)</f>
-        <v>260</v>
+        <v>350</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F14" ca="1" si="1">C2-E2-G2-H2</f>
-        <v>530</v>
+        <v>400</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G14" ca="1" si="2">ROUND((RANDBETWEEN(15,20)/100)*C2,0)</f>
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H14" ca="1" si="3">ROUND((RANDBETWEEN(5,10)/100)*C2,0)</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I2" s="6">
         <f t="shared" ref="I2:I14" ca="1" si="4">E2/$C2</f>
-        <v>0.26</v>
+        <v>0.35</v>
       </c>
       <c r="J2" s="6">
         <f t="shared" ref="J2:J14" ca="1" si="5">F2/$C2</f>
-        <v>0.53</v>
+        <v>0.4</v>
       </c>
       <c r="K2" s="6">
         <f t="shared" ref="K2:K14" ca="1" si="6">G2/$C2</f>
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="L2" s="6">
         <f t="shared" ref="L2:L14" ca="1" si="7">H2/$C2</f>
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="M2" s="7">
         <f t="shared" ref="M2:M14" ca="1" si="8">ROUND((RANDBETWEEN(20,60)/100)*C2,0)</f>
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="N2" s="7">
         <f t="shared" ref="N2:N14" ca="1" si="9">C2-M2</f>
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="O2" s="6">
         <f t="shared" ref="O2:O14" ca="1" si="10">M2/C2</f>
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="P2" s="6">
         <f t="shared" ref="P2:P14" ca="1" si="11">N2/C2</f>
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="Q2" s="5">
         <f t="shared" ref="Q2:Q14" ca="1" si="12">ROUND((RANDBETWEEN(10,40)/100)*C2,0)</f>
-        <v>140</v>
+        <v>260</v>
       </c>
       <c r="R2" s="5">
         <f t="shared" ref="R2:R14" ca="1" si="13">C2-Q2-S2</f>
-        <v>660</v>
+        <v>470</v>
       </c>
       <c r="S2" s="5">
         <f t="shared" ref="S2:S14" ca="1" si="14">ROUND((RANDBETWEEN(15,30)/100)*C2,0)</f>
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="T2" s="8">
         <f t="shared" ref="T2:T14" ca="1" si="15">Q2/C2</f>
-        <v>0.14000000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="U2" s="8">
         <f t="shared" ref="U2:U14" ca="1" si="16">R2/C2</f>
-        <v>0.66</v>
+        <v>0.47</v>
       </c>
       <c r="V2" s="8">
         <f t="shared" ref="V2:V14" ca="1" si="17">S2/C2</f>
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41812,15 +42563,15 @@
       </c>
       <c r="E3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>280</v>
+        <v>310</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ca="1" si="3"/>
@@ -41828,15 +42579,15 @@
       </c>
       <c r="I3" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="K3" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" ca="1" si="7"/>
@@ -41844,43 +42595,43 @@
       </c>
       <c r="M3" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="O3" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="P3" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="Q3" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="R3" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>470</v>
+        <v>740</v>
       </c>
       <c r="S3" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="T3" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.23</v>
+        <v>0.11</v>
       </c>
       <c r="U3" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.47</v>
+        <v>0.74</v>
       </c>
       <c r="V3" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -41899,59 +42650,59 @@
       </c>
       <c r="E4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>599</v>
+        <v>550</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="I4" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.29039999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="J4" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.47920000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="K4" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="L4" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>7.0400000000000004E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>425</v>
+        <v>288</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>825</v>
+        <v>962</v>
       </c>
       <c r="O4" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.34</v>
+        <v>0.23039999999999999</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.66</v>
+        <v>0.76959999999999995</v>
       </c>
       <c r="Q4" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>238</v>
+        <v>463</v>
       </c>
       <c r="R4" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>662</v>
+        <v>437</v>
       </c>
       <c r="S4" s="5">
         <f t="shared" ca="1" si="14"/>
@@ -41959,11 +42710,11 @@
       </c>
       <c r="T4" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.19040000000000001</v>
+        <v>0.37040000000000001</v>
       </c>
       <c r="U4" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.52959999999999996</v>
+        <v>0.34960000000000002</v>
       </c>
       <c r="V4" s="8">
         <f t="shared" ca="1" si="17"/>
@@ -41986,75 +42737,75 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>460</v>
+        <v>500</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="I5" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.28999999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.46</v>
+        <v>0.5</v>
       </c>
       <c r="K5" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>520</v>
+        <v>440</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>480</v>
+        <v>560</v>
       </c>
       <c r="O5" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.48</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="Q5" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="R5" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>430</v>
+        <v>330</v>
       </c>
       <c r="S5" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>210</v>
+        <v>270</v>
       </c>
       <c r="T5" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.36</v>
+        <v>0.4</v>
       </c>
       <c r="U5" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.43</v>
+        <v>0.33</v>
       </c>
       <c r="V5" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.21</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42077,15 +42828,15 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>552</v>
+        <v>564</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="I6" s="6">
         <f t="shared" ca="1" si="4"/>
@@ -42093,55 +42844,55 @@
       </c>
       <c r="J6" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="K6" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>924</v>
+        <v>912</v>
       </c>
       <c r="O6" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.77</v>
+        <v>0.76</v>
       </c>
       <c r="Q6" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>360</v>
+        <v>264</v>
       </c>
       <c r="R6" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>648</v>
+        <v>684</v>
       </c>
       <c r="S6" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>192</v>
+        <v>252</v>
       </c>
       <c r="T6" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="U6" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.54</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="V6" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42160,75 +42911,75 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.44</v>
+        <v>0.4</v>
       </c>
       <c r="K7" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>230</v>
+        <v>330</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>770</v>
+        <v>670</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.77</v>
+        <v>0.67</v>
       </c>
       <c r="Q7" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>340</v>
+        <v>100</v>
       </c>
       <c r="R7" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>380</v>
+        <v>600</v>
       </c>
       <c r="S7" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="T7" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.34</v>
+        <v>0.1</v>
       </c>
       <c r="U7" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.38</v>
+        <v>0.6</v>
       </c>
       <c r="V7" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42247,75 +42998,75 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>330</v>
+        <v>270</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.42</v>
+        <v>0.48</v>
       </c>
       <c r="K8" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>370</v>
+        <v>600</v>
       </c>
       <c r="N8" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>630</v>
+        <v>400</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.37</v>
+        <v>0.6</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.63</v>
+        <v>0.4</v>
       </c>
       <c r="Q8" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>190</v>
+        <v>340</v>
       </c>
       <c r="R8" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>660</v>
+        <v>440</v>
       </c>
       <c r="S8" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="T8" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.19</v>
+        <v>0.34</v>
       </c>
       <c r="U8" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.66</v>
+        <v>0.44</v>
       </c>
       <c r="V8" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.15</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42334,11 +43085,11 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" ca="1" si="2"/>
@@ -42346,15 +43097,15 @@
       </c>
       <c r="H9" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="K9" s="6">
         <f t="shared" ca="1" si="6"/>
@@ -42362,7 +43113,7 @@
       </c>
       <c r="L9" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -42382,27 +43133,27 @@
       </c>
       <c r="Q9" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="R9" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="S9" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="T9" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.13</v>
+        <v>0.26</v>
       </c>
       <c r="U9" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.57999999999999996</v>
+        <v>0.54</v>
       </c>
       <c r="V9" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.28999999999999998</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42421,15 +43172,15 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>380</v>
+        <v>410</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" ca="1" si="3"/>
@@ -42437,15 +43188,15 @@
       </c>
       <c r="I10" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.38</v>
+        <v>0.41</v>
       </c>
       <c r="K10" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" ca="1" si="7"/>
@@ -42453,43 +43204,43 @@
       </c>
       <c r="M10" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>250</v>
+        <v>530</v>
       </c>
       <c r="N10" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>750</v>
+        <v>470</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.25</v>
+        <v>0.53</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.75</v>
+        <v>0.47</v>
       </c>
       <c r="Q10" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>350</v>
+        <v>390</v>
       </c>
       <c r="R10" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>460</v>
+        <v>380</v>
       </c>
       <c r="S10" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="T10" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="U10" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.46</v>
+        <v>0.38</v>
       </c>
       <c r="V10" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.19</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42508,35 +43259,35 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>540</v>
+        <v>600</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>940</v>
+        <v>880</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27</v>
+        <v>0.3</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="K11" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="L11" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="8"/>
@@ -42556,27 +43307,27 @@
       </c>
       <c r="Q11" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="R11" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>780</v>
+        <v>960</v>
       </c>
       <c r="S11" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="T11" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="U11" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.39</v>
+        <v>0.48</v>
       </c>
       <c r="V11" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42595,11 +43346,11 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>490</v>
+        <v>470</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" ca="1" si="2"/>
@@ -42607,15 +43358,15 @@
       </c>
       <c r="H12" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.49</v>
+        <v>0.47</v>
       </c>
       <c r="K12" s="6">
         <f t="shared" ca="1" si="6"/>
@@ -42623,47 +43374,47 @@
       </c>
       <c r="L12" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>430</v>
+        <v>250</v>
       </c>
       <c r="N12" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>570</v>
+        <v>750</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.43</v>
+        <v>0.25</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.56999999999999995</v>
+        <v>0.75</v>
       </c>
       <c r="Q12" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="R12" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>560</v>
+        <v>610</v>
       </c>
       <c r="S12" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="T12" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.56000000000000005</v>
+        <v>0.61</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42682,51 +43433,51 @@
       </c>
       <c r="E13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>389</v>
+        <v>322</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.28000000000000003</v>
+        <v>0.33066666666666666</v>
       </c>
       <c r="J13" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.51866666666666672</v>
+        <v>0.42933333333333334</v>
       </c>
       <c r="K13" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.15066666666666667</v>
+        <v>0.16</v>
       </c>
       <c r="L13" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>5.0666666666666665E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M13" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>428</v>
+        <v>173</v>
       </c>
       <c r="N13" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>322</v>
+        <v>577</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.57066666666666666</v>
+        <v>0.23066666666666666</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.42933333333333334</v>
+        <v>0.76933333333333331</v>
       </c>
       <c r="Q13" s="5">
         <f t="shared" ca="1" si="12"/>
@@ -42734,11 +43485,11 @@
       </c>
       <c r="R13" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="S13" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="T13" s="8">
         <f t="shared" ca="1" si="15"/>
@@ -42746,11 +43497,11 @@
       </c>
       <c r="U13" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.65866666666666662</v>
+        <v>0.66933333333333334</v>
       </c>
       <c r="V13" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.17066666666666666</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -42769,75 +43520,75 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>250</v>
+        <v>290</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>460</v>
+        <v>510</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.25</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J14" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.46</v>
+        <v>0.51</v>
       </c>
       <c r="K14" s="6">
         <f t="shared" ca="1" si="6"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" ca="1" si="7"/>
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="M14" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>570</v>
+        <v>440</v>
       </c>
       <c r="N14" s="7">
         <f t="shared" ca="1" si="9"/>
-        <v>430</v>
+        <v>560</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>0.56999999999999995</v>
+        <v>0.44</v>
       </c>
       <c r="P14" s="6">
         <f t="shared" ca="1" si="11"/>
-        <v>0.43</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="Q14" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>140</v>
+        <v>400</v>
       </c>
       <c r="R14" s="5">
         <f t="shared" ca="1" si="13"/>
-        <v>700</v>
+        <v>390</v>
       </c>
       <c r="S14" s="5">
         <f t="shared" ca="1" si="14"/>
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="T14" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>0.14000000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="U14" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>0.7</v>
+        <v>0.39</v>
       </c>
       <c r="V14" s="8">
         <f t="shared" ca="1" si="17"/>
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>